<commit_message>
Update my logbook with changing aircraft type to ICAO one.
</commit_message>
<xml_diff>
--- a/My_Flying_Logbook.xlsx
+++ b/My_Flying_Logbook.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haoren/Documents/PA28/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67A220B7-4265-0F4B-96EB-3D3C2814DA54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A54CB70E-E358-D242-A4A0-08DD01CB6BD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="4" xr2:uid="{634C8D91-949A-EA46-A557-4B6714D72E97}"/>
   </bookViews>
@@ -110,9 +110,6 @@
     <t>April</t>
   </si>
   <si>
-    <t>PA-28</t>
-  </si>
-  <si>
     <t>VH-LXP</t>
   </si>
   <si>
@@ -381,6 +378,9 @@
   </si>
   <si>
     <t>YSBK-LOE-LRF-LOE-YSBK</t>
+  </si>
+  <si>
+    <t>P28A</t>
   </si>
 </sst>
 </file>
@@ -933,7 +933,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1079,6 +1079,63 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1100,61 +1157,43 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1181,43 +1220,7 @@
     <xf numFmtId="164" fontId="1" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1509,15 +1512,15 @@
     <row r="1" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:4" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C3" s="23">
         <v>1127225</v>
@@ -1526,13 +1529,13 @@
     <row r="4" spans="2:4" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="2:4" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="D5" s="29" t="s">
         <v>41</v>
-      </c>
-      <c r="D5" s="29" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -1540,10 +1543,10 @@
         <v>44308</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="31" t="s">
         <v>43</v>
-      </c>
-      <c r="D6" s="31" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -1551,10 +1554,10 @@
         <v>44575</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -1678,98 +1681,98 @@
   <sheetData>
     <row r="1" spans="2:29" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B2" s="67" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68" t="s">
+      <c r="B2" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="68"/>
-      <c r="F2" s="71" t="s">
+      <c r="E2" s="53"/>
+      <c r="F2" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="71" t="s">
+      <c r="G2" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="68" t="s">
+      <c r="H2" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="68"/>
-      <c r="J2" s="68"/>
-      <c r="K2" s="64" t="s">
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="65"/>
-      <c r="M2" s="66"/>
-      <c r="N2" s="59" t="s">
+      <c r="L2" s="50"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="59"/>
-      <c r="P2" s="59"/>
-      <c r="Q2" s="59"/>
-      <c r="R2" s="59"/>
-      <c r="S2" s="59"/>
-      <c r="T2" s="59" t="s">
+      <c r="O2" s="63"/>
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63"/>
+      <c r="R2" s="63"/>
+      <c r="S2" s="63"/>
+      <c r="T2" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="U2" s="59"/>
-      <c r="V2" s="59"/>
-      <c r="W2" s="59"/>
-      <c r="X2" s="59"/>
-      <c r="Y2" s="59"/>
-      <c r="Z2" s="60"/>
-      <c r="AA2" s="61"/>
-      <c r="AB2" s="59" t="s">
+      <c r="U2" s="63"/>
+      <c r="V2" s="63"/>
+      <c r="W2" s="63"/>
+      <c r="X2" s="63"/>
+      <c r="Y2" s="63"/>
+      <c r="Z2" s="64"/>
+      <c r="AA2" s="65"/>
+      <c r="AB2" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="AC2" s="62"/>
+      <c r="AC2" s="66"/>
     </row>
     <row r="3" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B3" s="69"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="70"/>
-      <c r="I3" s="70"/>
-      <c r="J3" s="70"/>
-      <c r="K3" s="70"/>
-      <c r="L3" s="70"/>
-      <c r="M3" s="70"/>
-      <c r="N3" s="56" t="s">
+      <c r="B3" s="54"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="O3" s="56"/>
-      <c r="P3" s="56" t="s">
+      <c r="O3" s="60"/>
+      <c r="P3" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="Q3" s="56"/>
-      <c r="R3" s="56" t="s">
+      <c r="Q3" s="60"/>
+      <c r="R3" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="S3" s="56"/>
-      <c r="T3" s="56" t="s">
+      <c r="S3" s="60"/>
+      <c r="T3" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="U3" s="56"/>
-      <c r="V3" s="56" t="s">
+      <c r="U3" s="60"/>
+      <c r="V3" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="W3" s="56"/>
-      <c r="X3" s="56" t="s">
+      <c r="W3" s="60"/>
+      <c r="X3" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="Y3" s="56"/>
-      <c r="Z3" s="56" t="s">
+      <c r="Y3" s="60"/>
+      <c r="Z3" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="AA3" s="56"/>
-      <c r="AB3" s="56" t="s">
+      <c r="AA3" s="60"/>
+      <c r="AB3" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="AC3" s="57" t="s">
+      <c r="AC3" s="61" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1786,20 +1789,20 @@
       <c r="E4" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="73"/>
-      <c r="G4" s="73"/>
+      <c r="F4" s="58"/>
+      <c r="G4" s="58"/>
       <c r="H4" s="21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I4" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="J4" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="K4" s="74"/>
-      <c r="L4" s="74"/>
-      <c r="M4" s="74"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="59"/>
+      <c r="M4" s="59"/>
       <c r="N4" s="20" t="s">
         <v>10</v>
       </c>
@@ -1842,8 +1845,8 @@
       <c r="AA4" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="AB4" s="63"/>
-      <c r="AC4" s="58"/>
+      <c r="AB4" s="67"/>
+      <c r="AC4" s="62"/>
     </row>
     <row r="5" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B5" s="37" t="s">
@@ -1853,25 +1856,25 @@
         <v>24</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="I5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
@@ -1900,26 +1903,26 @@
       <c r="C6" s="13">
         <v>29</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E6" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="F6" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="G6" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="13" t="s">
-        <v>25</v>
-      </c>
       <c r="H6" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K6" s="11"/>
       <c r="L6" s="11"/>
@@ -1948,26 +1951,26 @@
       <c r="C7" s="13">
         <v>30</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E7" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="F7" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="G7" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="13" t="s">
-        <v>25</v>
-      </c>
       <c r="H7" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K7" s="11"/>
       <c r="L7" s="11"/>
@@ -1996,26 +1999,26 @@
       <c r="C8" s="13">
         <v>30</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E8" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="F8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="G8" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="13" t="s">
-        <v>25</v>
-      </c>
       <c r="H8" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K8" s="11"/>
       <c r="L8" s="11"/>
@@ -2044,26 +2047,26 @@
       <c r="C9" s="13">
         <v>31</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="F9" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="G9" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="G9" s="13" t="s">
-        <v>25</v>
-      </c>
       <c r="H9" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K9" s="11"/>
       <c r="L9" s="11"/>
@@ -2094,26 +2097,26 @@
       <c r="C10" s="13">
         <v>1</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E10" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="F10" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="G10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="13" t="s">
-        <v>25</v>
-      </c>
       <c r="H10" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I10" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J10" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K10" s="11"/>
       <c r="L10" s="11"/>
@@ -2142,26 +2145,26 @@
       <c r="C11" s="13">
         <v>7</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E11" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="F11" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="G11" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="13" t="s">
-        <v>25</v>
-      </c>
       <c r="H11" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I11" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J11" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K11" s="11"/>
       <c r="L11" s="11"/>
@@ -2190,26 +2193,26 @@
       <c r="C12" s="13">
         <v>8</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E12" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="F12" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="G12" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="13" t="s">
-        <v>25</v>
-      </c>
       <c r="H12" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I12" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J12" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K12" s="11"/>
       <c r="L12" s="11"/>
@@ -2238,26 +2241,26 @@
       <c r="C13" s="13">
         <v>8</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E13" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="F13" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="13" t="s">
+      <c r="G13" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="13" t="s">
-        <v>25</v>
-      </c>
       <c r="H13" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I13" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J13" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K13" s="11"/>
       <c r="L13" s="11"/>
@@ -2286,26 +2289,26 @@
       <c r="C14" s="13">
         <v>9</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E14" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="F14" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="13" t="s">
+      <c r="G14" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="13" t="s">
-        <v>25</v>
-      </c>
       <c r="H14" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I14" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J14" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K14" s="11"/>
       <c r="L14" s="11"/>
@@ -2334,26 +2337,26 @@
       <c r="C15" s="13">
         <v>9</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E15" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="F15" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="13" t="s">
+      <c r="G15" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="G15" s="13" t="s">
-        <v>25</v>
-      </c>
       <c r="H15" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I15" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K15" s="11"/>
       <c r="L15" s="11"/>
@@ -2382,26 +2385,26 @@
       <c r="C16" s="13">
         <v>12</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E16" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="F16" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="13" t="s">
+      <c r="G16" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="G16" s="13" t="s">
-        <v>25</v>
-      </c>
       <c r="H16" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I16" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J16" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K16" s="11"/>
       <c r="L16" s="11"/>
@@ -2430,26 +2433,26 @@
       <c r="C17" s="13">
         <v>13</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E17" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="F17" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F17" s="13" t="s">
+      <c r="G17" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="G17" s="13" t="s">
-        <v>25</v>
-      </c>
       <c r="H17" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J17" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K17" s="11"/>
       <c r="L17" s="11"/>
@@ -2478,26 +2481,26 @@
       <c r="C18" s="13">
         <v>14</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E18" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="13" t="s">
+      <c r="F18" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F18" s="13" t="s">
+      <c r="G18" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="G18" s="13" t="s">
-        <v>25</v>
-      </c>
       <c r="H18" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I18" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J18" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K18" s="11"/>
       <c r="L18" s="11"/>
@@ -2526,26 +2529,26 @@
       <c r="C19" s="13">
         <v>20</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E19" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="F19" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F19" s="13" t="s">
+      <c r="G19" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="G19" s="13" t="s">
-        <v>25</v>
-      </c>
       <c r="H19" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I19" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J19" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K19" s="11"/>
       <c r="L19" s="11"/>
@@ -2574,26 +2577,26 @@
       <c r="C20" s="13">
         <v>20</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E20" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E20" s="13" t="s">
+      <c r="F20" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="13" t="s">
+      <c r="G20" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="G20" s="13" t="s">
-        <v>25</v>
-      </c>
       <c r="H20" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I20" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J20" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K20" s="11"/>
       <c r="L20" s="11"/>
@@ -2622,26 +2625,26 @@
       <c r="C21" s="13">
         <v>28</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="D21" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E21" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="13" t="s">
+      <c r="F21" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F21" s="13" t="s">
+      <c r="G21" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="G21" s="13" t="s">
-        <v>25</v>
-      </c>
       <c r="H21" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I21" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J21" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K21" s="11"/>
       <c r="L21" s="11"/>
@@ -2670,26 +2673,26 @@
       <c r="C22" s="13">
         <v>29</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D22" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E22" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="13" t="s">
+      <c r="F22" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F22" s="13" t="s">
+      <c r="G22" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="G22" s="13" t="s">
-        <v>25</v>
-      </c>
       <c r="H22" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I22" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J22" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K22" s="11"/>
       <c r="L22" s="11"/>
@@ -2715,31 +2718,31 @@
     </row>
     <row r="23" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B23" s="32" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C23" s="13">
         <v>10</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E23" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E23" s="13" t="s">
+      <c r="F23" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F23" s="13" t="s">
+      <c r="G23" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="G23" s="13" t="s">
-        <v>25</v>
-      </c>
       <c r="H23" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I23" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J23" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K23" s="11"/>
       <c r="L23" s="11"/>
@@ -2768,26 +2771,26 @@
       <c r="C24" s="15">
         <v>10</v>
       </c>
-      <c r="D24" s="15" t="s">
+      <c r="D24" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E24" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="E24" s="15" t="s">
-        <v>23</v>
-      </c>
       <c r="F24" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G24" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H24" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I24" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J24" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K24" s="16"/>
       <c r="L24" s="16"/>
@@ -2816,26 +2819,26 @@
       <c r="C25" s="14">
         <v>25</v>
       </c>
-      <c r="D25" s="14" t="s">
+      <c r="D25" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E25" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="E25" s="14" t="s">
+      <c r="F25" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F25" s="14" t="s">
+      <c r="G25" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="G25" s="14" t="s">
-        <v>25</v>
-      </c>
       <c r="H25" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I25" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J25" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K25" s="12"/>
       <c r="L25" s="12"/>
@@ -2860,22 +2863,22 @@
       <c r="AC25" s="42"/>
     </row>
     <row r="26" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B26" s="49" t="s">
-        <v>62</v>
-      </c>
-      <c r="C26" s="50"/>
-      <c r="D26" s="50"/>
-      <c r="E26" s="50"/>
-      <c r="F26" s="50"/>
+      <c r="B26" s="68" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="69"/>
+      <c r="D26" s="69"/>
+      <c r="E26" s="69"/>
+      <c r="F26" s="69"/>
       <c r="G26" s="18">
         <f>IF(SUM(K26:AA26)=0,"",SUM(K26:AA26))</f>
         <v>23.499999999999996</v>
       </c>
-      <c r="H26" s="50" t="s">
-        <v>49</v>
-      </c>
-      <c r="I26" s="50"/>
-      <c r="J26" s="50"/>
+      <c r="H26" s="69" t="s">
+        <v>48</v>
+      </c>
+      <c r="I26" s="69"/>
+      <c r="J26" s="69"/>
       <c r="K26" s="18" t="str">
         <f>IF(SUM(K5:K25)=0,"",SUM(K5:K25))</f>
         <v/>
@@ -2954,22 +2957,22 @@
       </c>
     </row>
     <row r="27" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B27" s="51" t="s">
-        <v>63</v>
-      </c>
-      <c r="C27" s="52"/>
-      <c r="D27" s="52"/>
-      <c r="E27" s="52"/>
-      <c r="F27" s="52"/>
+      <c r="B27" s="70" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" s="71"/>
+      <c r="D27" s="71"/>
+      <c r="E27" s="71"/>
+      <c r="F27" s="71"/>
       <c r="G27" s="19">
         <f>IF(SUM(K28:AA28)=0,"",SUM(K28:AA28))</f>
         <v>23.499999999999996</v>
       </c>
-      <c r="H27" s="55" t="s">
-        <v>61</v>
-      </c>
-      <c r="I27" s="55"/>
-      <c r="J27" s="55"/>
+      <c r="H27" s="74" t="s">
+        <v>60</v>
+      </c>
+      <c r="I27" s="74"/>
+      <c r="J27" s="74"/>
       <c r="K27" s="19"/>
       <c r="L27" s="19"/>
       <c r="M27" s="19"/>
@@ -2991,22 +2994,22 @@
       <c r="AC27" s="44"/>
     </row>
     <row r="28" spans="2:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="53" t="s">
-        <v>64</v>
-      </c>
-      <c r="C28" s="54"/>
-      <c r="D28" s="54"/>
-      <c r="E28" s="54"/>
-      <c r="F28" s="54"/>
+      <c r="B28" s="72" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="73"/>
+      <c r="D28" s="73"/>
+      <c r="E28" s="73"/>
+      <c r="F28" s="73"/>
       <c r="G28" s="45">
         <f>IF(SUM(G27,AC28)=0, "", SUM(G27,AC28))</f>
         <v>23.499999999999996</v>
       </c>
-      <c r="H28" s="54" t="s">
-        <v>50</v>
-      </c>
-      <c r="I28" s="54"/>
-      <c r="J28" s="54"/>
+      <c r="H28" s="73" t="s">
+        <v>49</v>
+      </c>
+      <c r="I28" s="73"/>
+      <c r="J28" s="73"/>
       <c r="K28" s="45" t="str">
         <f>IF(SUM(K26:K27)=0,"",SUM(K26:K27))</f>
         <v/>
@@ -3086,15 +3089,12 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="D2:E3"/>
-    <mergeCell ref="F2:F4"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="H2:J3"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="H26:J26"/>
+    <mergeCell ref="H27:J27"/>
+    <mergeCell ref="H28:J28"/>
     <mergeCell ref="N3:O3"/>
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="AC3:AC4"/>
@@ -3108,12 +3108,15 @@
     <mergeCell ref="X3:Y3"/>
     <mergeCell ref="Z3:AA3"/>
     <mergeCell ref="AB3:AB4"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="H26:J26"/>
-    <mergeCell ref="H27:J27"/>
-    <mergeCell ref="H28:J28"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="D2:E3"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="H2:J3"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="M3:M4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="86" fitToWidth="2" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
@@ -3147,98 +3150,98 @@
   <sheetData>
     <row r="1" spans="2:29" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B2" s="83" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="84"/>
-      <c r="D2" s="87" t="s">
+      <c r="B2" s="75" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="76"/>
+      <c r="D2" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="84"/>
-      <c r="F2" s="89" t="s">
+      <c r="E2" s="76"/>
+      <c r="F2" s="81" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="89" t="s">
+      <c r="G2" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="87" t="s">
+      <c r="H2" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="92"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="64" t="s">
+      <c r="I2" s="84"/>
+      <c r="J2" s="76"/>
+      <c r="K2" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="65"/>
-      <c r="M2" s="66"/>
-      <c r="N2" s="60" t="s">
+      <c r="L2" s="50"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="79"/>
-      <c r="P2" s="79"/>
-      <c r="Q2" s="79"/>
-      <c r="R2" s="79"/>
-      <c r="S2" s="61"/>
-      <c r="T2" s="60" t="s">
+      <c r="O2" s="92"/>
+      <c r="P2" s="92"/>
+      <c r="Q2" s="92"/>
+      <c r="R2" s="92"/>
+      <c r="S2" s="65"/>
+      <c r="T2" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="U2" s="79"/>
-      <c r="V2" s="79"/>
-      <c r="W2" s="79"/>
-      <c r="X2" s="79"/>
-      <c r="Y2" s="61"/>
-      <c r="Z2" s="60"/>
-      <c r="AA2" s="61"/>
-      <c r="AB2" s="60" t="s">
+      <c r="U2" s="92"/>
+      <c r="V2" s="92"/>
+      <c r="W2" s="92"/>
+      <c r="X2" s="92"/>
+      <c r="Y2" s="65"/>
+      <c r="Z2" s="64"/>
+      <c r="AA2" s="65"/>
+      <c r="AB2" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="AC2" s="80"/>
+      <c r="AC2" s="93"/>
     </row>
     <row r="3" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B3" s="85"/>
-      <c r="C3" s="86"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="88"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="86"/>
-      <c r="K3" s="94"/>
-      <c r="L3" s="94"/>
-      <c r="M3" s="94"/>
-      <c r="N3" s="75" t="s">
+      <c r="B3" s="77"/>
+      <c r="C3" s="78"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="78"/>
+      <c r="K3" s="86"/>
+      <c r="L3" s="86"/>
+      <c r="M3" s="86"/>
+      <c r="N3" s="88" t="s">
         <v>9</v>
       </c>
-      <c r="O3" s="76"/>
-      <c r="P3" s="75" t="s">
+      <c r="O3" s="89"/>
+      <c r="P3" s="88" t="s">
         <v>12</v>
       </c>
-      <c r="Q3" s="76"/>
-      <c r="R3" s="75" t="s">
+      <c r="Q3" s="89"/>
+      <c r="R3" s="88" t="s">
         <v>13</v>
       </c>
-      <c r="S3" s="76"/>
-      <c r="T3" s="75" t="s">
+      <c r="S3" s="89"/>
+      <c r="T3" s="88" t="s">
         <v>9</v>
       </c>
-      <c r="U3" s="76"/>
-      <c r="V3" s="75" t="s">
+      <c r="U3" s="89"/>
+      <c r="V3" s="88" t="s">
         <v>12</v>
       </c>
-      <c r="W3" s="76"/>
-      <c r="X3" s="75" t="s">
+      <c r="W3" s="89"/>
+      <c r="X3" s="88" t="s">
         <v>13</v>
       </c>
-      <c r="Y3" s="76"/>
-      <c r="Z3" s="75" t="s">
+      <c r="Y3" s="89"/>
+      <c r="Z3" s="88" t="s">
         <v>16</v>
       </c>
-      <c r="AA3" s="76"/>
-      <c r="AB3" s="81" t="s">
+      <c r="AA3" s="89"/>
+      <c r="AB3" s="94" t="s">
         <v>18</v>
       </c>
-      <c r="AC3" s="77" t="s">
+      <c r="AC3" s="90" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3255,20 +3258,20 @@
       <c r="E4" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="91"/>
-      <c r="G4" s="91"/>
+      <c r="F4" s="83"/>
+      <c r="G4" s="83"/>
       <c r="H4" s="21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I4" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="J4" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="K4" s="95"/>
-      <c r="L4" s="95"/>
-      <c r="M4" s="95"/>
+      <c r="K4" s="87"/>
+      <c r="L4" s="87"/>
+      <c r="M4" s="87"/>
       <c r="N4" s="20" t="s">
         <v>10</v>
       </c>
@@ -3311,36 +3314,36 @@
       <c r="AA4" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="AB4" s="82"/>
-      <c r="AC4" s="78"/>
+      <c r="AB4" s="95"/>
+      <c r="AC4" s="91"/>
     </row>
     <row r="5" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B5" s="37" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C5" s="1">
         <v>31</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="H5" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -3369,26 +3372,26 @@
       <c r="C6" s="8">
         <v>31</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="96" t="s">
+        <v>100</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>23</v>
-      </c>
       <c r="F6" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K6" s="8"/>
       <c r="L6" s="8"/>
@@ -3414,31 +3417,31 @@
     </row>
     <row r="7" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B7" s="32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C7" s="13">
         <v>2</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E7" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="F7" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="G7" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="13" t="s">
-        <v>25</v>
-      </c>
       <c r="H7" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K7" s="13"/>
       <c r="L7" s="13"/>
@@ -3468,25 +3471,25 @@
         <v>22</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="H8" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
@@ -3515,26 +3518,26 @@
       <c r="C9" s="13">
         <v>22</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="13" t="s">
-        <v>23</v>
-      </c>
       <c r="F9" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K9" s="13"/>
       <c r="L9" s="13"/>
@@ -3560,31 +3563,31 @@
     </row>
     <row r="10" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B10" s="37" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C10" s="1">
         <v>6</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="H10" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
@@ -3613,26 +3616,26 @@
       <c r="C11" s="13">
         <v>6</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E11" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="13" t="s">
-        <v>23</v>
-      </c>
       <c r="F11" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I11" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J11" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K11" s="13"/>
       <c r="L11" s="13"/>
@@ -3658,31 +3661,31 @@
     </row>
     <row r="12" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B12" s="32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C12" s="13">
         <v>4</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E12" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="13" t="s">
-        <v>23</v>
-      </c>
       <c r="F12" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I12" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J12" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K12" s="13"/>
       <c r="L12" s="13"/>
@@ -3711,26 +3714,26 @@
       <c r="C13" s="14">
         <v>9</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E13" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="14" t="s">
-        <v>23</v>
-      </c>
       <c r="F13" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I13" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J13" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K13" s="14"/>
       <c r="L13" s="14"/>
@@ -4115,22 +4118,22 @@
       <c r="AC25" s="42"/>
     </row>
     <row r="26" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B26" s="49" t="s">
-        <v>62</v>
-      </c>
-      <c r="C26" s="50"/>
-      <c r="D26" s="50"/>
-      <c r="E26" s="50"/>
-      <c r="F26" s="50"/>
+      <c r="B26" s="68" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="69"/>
+      <c r="D26" s="69"/>
+      <c r="E26" s="69"/>
+      <c r="F26" s="69"/>
       <c r="G26" s="18">
         <f>IF(SUM(K26:AA26)=0,"",SUM(K26:AA26))</f>
         <v>6.7999999999999989</v>
       </c>
-      <c r="H26" s="50" t="s">
-        <v>49</v>
-      </c>
-      <c r="I26" s="50"/>
-      <c r="J26" s="50"/>
+      <c r="H26" s="69" t="s">
+        <v>48</v>
+      </c>
+      <c r="I26" s="69"/>
+      <c r="J26" s="69"/>
       <c r="K26" s="18" t="str">
         <f>IF(SUM(K5:K25)=0,"",SUM(K5:K25))</f>
         <v/>
@@ -4209,22 +4212,22 @@
       </c>
     </row>
     <row r="27" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B27" s="51" t="s">
-        <v>63</v>
-      </c>
-      <c r="C27" s="52"/>
-      <c r="D27" s="52"/>
-      <c r="E27" s="52"/>
-      <c r="F27" s="52"/>
+      <c r="B27" s="70" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" s="71"/>
+      <c r="D27" s="71"/>
+      <c r="E27" s="71"/>
+      <c r="F27" s="71"/>
       <c r="G27" s="19">
         <f>IF(SUM(K28:AA28)=0,"",SUM(K28:AA28))</f>
         <v>30.299999999999997</v>
       </c>
-      <c r="H27" s="55" t="s">
-        <v>61</v>
-      </c>
-      <c r="I27" s="55"/>
-      <c r="J27" s="55"/>
+      <c r="H27" s="74" t="s">
+        <v>60</v>
+      </c>
+      <c r="I27" s="74"/>
+      <c r="J27" s="74"/>
       <c r="K27" s="19" t="str">
         <f>'Page 01'!K28</f>
         <v/>
@@ -4303,22 +4306,22 @@
       </c>
     </row>
     <row r="28" spans="2:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="53" t="s">
-        <v>64</v>
-      </c>
-      <c r="C28" s="54"/>
-      <c r="D28" s="54"/>
-      <c r="E28" s="54"/>
-      <c r="F28" s="54"/>
+      <c r="B28" s="72" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="73"/>
+      <c r="D28" s="73"/>
+      <c r="E28" s="73"/>
+      <c r="F28" s="73"/>
       <c r="G28" s="45">
         <f>IF(SUM(G27,AC28)=0, "", SUM(G27,AC28))</f>
         <v>30.299999999999997</v>
       </c>
-      <c r="H28" s="54" t="s">
-        <v>50</v>
-      </c>
-      <c r="I28" s="54"/>
-      <c r="J28" s="54"/>
+      <c r="H28" s="73" t="s">
+        <v>49</v>
+      </c>
+      <c r="I28" s="73"/>
+      <c r="J28" s="73"/>
       <c r="K28" s="45" t="str">
         <f>IF(SUM(K26:K27)=0,"",SUM(K26:K27))</f>
         <v/>
@@ -4398,15 +4401,12 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="D2:E3"/>
-    <mergeCell ref="F2:F4"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="H2:J3"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="H26:J26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="H27:J27"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="H28:J28"/>
     <mergeCell ref="N3:O3"/>
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="AC3:AC4"/>
@@ -4420,12 +4420,15 @@
     <mergeCell ref="X3:Y3"/>
     <mergeCell ref="Z3:AA3"/>
     <mergeCell ref="AB3:AB4"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="H26:J26"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="H27:J27"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="H28:J28"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="D2:E3"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="H2:J3"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="M3:M4"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4441,9 +4444,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="B1:AC28"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4462,98 +4463,98 @@
   <sheetData>
     <row r="1" spans="2:29" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B2" s="83" t="s">
-        <v>81</v>
-      </c>
-      <c r="C2" s="84"/>
-      <c r="D2" s="87" t="s">
+      <c r="B2" s="75" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="76"/>
+      <c r="D2" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="84"/>
-      <c r="F2" s="89" t="s">
+      <c r="E2" s="76"/>
+      <c r="F2" s="81" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="89" t="s">
+      <c r="G2" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="87" t="s">
+      <c r="H2" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="92"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="64" t="s">
+      <c r="I2" s="84"/>
+      <c r="J2" s="76"/>
+      <c r="K2" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="65"/>
-      <c r="M2" s="66"/>
-      <c r="N2" s="60" t="s">
+      <c r="L2" s="50"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="79"/>
-      <c r="P2" s="79"/>
-      <c r="Q2" s="79"/>
-      <c r="R2" s="79"/>
-      <c r="S2" s="61"/>
-      <c r="T2" s="60" t="s">
+      <c r="O2" s="92"/>
+      <c r="P2" s="92"/>
+      <c r="Q2" s="92"/>
+      <c r="R2" s="92"/>
+      <c r="S2" s="65"/>
+      <c r="T2" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="U2" s="79"/>
-      <c r="V2" s="79"/>
-      <c r="W2" s="79"/>
-      <c r="X2" s="79"/>
-      <c r="Y2" s="61"/>
-      <c r="Z2" s="60"/>
-      <c r="AA2" s="61"/>
-      <c r="AB2" s="60" t="s">
+      <c r="U2" s="92"/>
+      <c r="V2" s="92"/>
+      <c r="W2" s="92"/>
+      <c r="X2" s="92"/>
+      <c r="Y2" s="65"/>
+      <c r="Z2" s="64"/>
+      <c r="AA2" s="65"/>
+      <c r="AB2" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="AC2" s="80"/>
+      <c r="AC2" s="93"/>
     </row>
     <row r="3" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B3" s="85"/>
-      <c r="C3" s="86"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="88"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="86"/>
-      <c r="K3" s="94"/>
-      <c r="L3" s="94"/>
-      <c r="M3" s="94"/>
-      <c r="N3" s="75" t="s">
+      <c r="B3" s="77"/>
+      <c r="C3" s="78"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="78"/>
+      <c r="K3" s="86"/>
+      <c r="L3" s="86"/>
+      <c r="M3" s="86"/>
+      <c r="N3" s="88" t="s">
         <v>9</v>
       </c>
-      <c r="O3" s="76"/>
-      <c r="P3" s="75" t="s">
+      <c r="O3" s="89"/>
+      <c r="P3" s="88" t="s">
         <v>12</v>
       </c>
-      <c r="Q3" s="76"/>
-      <c r="R3" s="75" t="s">
+      <c r="Q3" s="89"/>
+      <c r="R3" s="88" t="s">
         <v>13</v>
       </c>
-      <c r="S3" s="76"/>
-      <c r="T3" s="75" t="s">
+      <c r="S3" s="89"/>
+      <c r="T3" s="88" t="s">
         <v>9</v>
       </c>
-      <c r="U3" s="76"/>
-      <c r="V3" s="75" t="s">
+      <c r="U3" s="89"/>
+      <c r="V3" s="88" t="s">
         <v>12</v>
       </c>
-      <c r="W3" s="76"/>
-      <c r="X3" s="75" t="s">
+      <c r="W3" s="89"/>
+      <c r="X3" s="88" t="s">
         <v>13</v>
       </c>
-      <c r="Y3" s="76"/>
-      <c r="Z3" s="75" t="s">
+      <c r="Y3" s="89"/>
+      <c r="Z3" s="88" t="s">
         <v>16</v>
       </c>
-      <c r="AA3" s="76"/>
-      <c r="AB3" s="81" t="s">
+      <c r="AA3" s="89"/>
+      <c r="AB3" s="94" t="s">
         <v>18</v>
       </c>
-      <c r="AC3" s="77" t="s">
+      <c r="AC3" s="90" t="s">
         <v>19</v>
       </c>
     </row>
@@ -4570,20 +4571,20 @@
       <c r="E4" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="91"/>
-      <c r="G4" s="91"/>
+      <c r="F4" s="83"/>
+      <c r="G4" s="83"/>
       <c r="H4" s="21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I4" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="J4" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="K4" s="95"/>
-      <c r="L4" s="95"/>
-      <c r="M4" s="95"/>
+      <c r="K4" s="87"/>
+      <c r="L4" s="87"/>
+      <c r="M4" s="87"/>
       <c r="N4" s="20" t="s">
         <v>10</v>
       </c>
@@ -4626,36 +4627,36 @@
       <c r="AA4" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="AB4" s="82"/>
-      <c r="AC4" s="78"/>
+      <c r="AB4" s="95"/>
+      <c r="AC4" s="91"/>
     </row>
     <row r="5" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B5" s="37" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C5" s="1">
         <v>14</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="F5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="I5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -4685,25 +4686,25 @@
         <v>15</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="F6" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K6" s="13"/>
       <c r="L6" s="13"/>
@@ -4732,26 +4733,26 @@
       <c r="C7" s="13">
         <v>21</v>
       </c>
-      <c r="D7" s="13" t="s">
-        <v>22</v>
+      <c r="D7" s="1" t="s">
+        <v>100</v>
       </c>
       <c r="E7" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" s="13" t="s">
-        <v>72</v>
-      </c>
       <c r="I7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K7" s="13"/>
       <c r="L7" s="13"/>
@@ -4780,26 +4781,26 @@
       <c r="C8" s="13">
         <v>26</v>
       </c>
-      <c r="D8" s="13" t="s">
-        <v>22</v>
+      <c r="D8" s="1" t="s">
+        <v>100</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K8" s="13"/>
       <c r="L8" s="13"/>
@@ -4830,26 +4831,26 @@
       <c r="C9" s="13">
         <v>29</v>
       </c>
-      <c r="D9" s="13" t="s">
-        <v>22</v>
+      <c r="D9" s="1" t="s">
+        <v>100</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K9" s="13"/>
       <c r="L9" s="13"/>
@@ -4875,31 +4876,31 @@
     </row>
     <row r="10" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B10" s="32" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C10" s="13">
         <v>9</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E10" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="13" t="s">
-        <v>23</v>
-      </c>
       <c r="F10" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K10" s="13"/>
       <c r="L10" s="13"/>
@@ -4928,26 +4929,26 @@
       <c r="C11" s="13">
         <v>10</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E11" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="13" t="s">
-        <v>23</v>
-      </c>
       <c r="F11" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K11" s="13"/>
       <c r="L11" s="13"/>
@@ -4976,26 +4977,26 @@
       <c r="C12" s="13">
         <v>10</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E12" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="13" t="s">
-        <v>23</v>
-      </c>
       <c r="F12" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K12" s="13"/>
       <c r="L12" s="13"/>
@@ -5024,26 +5025,26 @@
       <c r="C13" s="13">
         <v>13</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E13" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="13" t="s">
-        <v>23</v>
-      </c>
       <c r="F13" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K13" s="13"/>
       <c r="L13" s="13"/>
@@ -5074,26 +5075,26 @@
       <c r="C14" s="13">
         <v>11</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E14" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="13" t="s">
-        <v>23</v>
-      </c>
       <c r="F14" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H14" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K14" s="13"/>
       <c r="L14" s="13"/>
@@ -5122,26 +5123,26 @@
       <c r="C15" s="13">
         <v>16</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E15" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="13" t="s">
-        <v>23</v>
-      </c>
       <c r="F15" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K15" s="13"/>
       <c r="L15" s="13"/>
@@ -5170,26 +5171,26 @@
       <c r="C16" s="13">
         <v>18</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E16" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="13" t="s">
-        <v>23</v>
-      </c>
       <c r="F16" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K16" s="13"/>
       <c r="L16" s="13"/>
@@ -5218,26 +5219,26 @@
       <c r="C17" s="13">
         <v>21</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E17" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E17" s="13" t="s">
-        <v>23</v>
-      </c>
       <c r="F17" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K17" s="13"/>
       <c r="L17" s="13"/>
@@ -5266,26 +5267,26 @@
       <c r="C18" s="13">
         <v>23</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E18" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="13" t="s">
-        <v>23</v>
-      </c>
       <c r="F18" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K18" s="13"/>
       <c r="L18" s="13"/>
@@ -5314,26 +5315,26 @@
       <c r="C19" s="13">
         <v>30</v>
       </c>
-      <c r="D19" s="13" t="s">
-        <v>22</v>
+      <c r="D19" s="1" t="s">
+        <v>100</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K19" s="13"/>
       <c r="L19" s="13"/>
@@ -5364,26 +5365,26 @@
       <c r="C20" s="13">
         <v>3</v>
       </c>
-      <c r="D20" s="13" t="s">
-        <v>22</v>
+      <c r="D20" s="1" t="s">
+        <v>100</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H20" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K20" s="13"/>
       <c r="L20" s="13"/>
@@ -5409,31 +5410,31 @@
     </row>
     <row r="21" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B21" s="32" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C21" s="13">
         <v>4</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="D21" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E21" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="13" t="s">
-        <v>23</v>
-      </c>
       <c r="F21" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K21" s="13"/>
       <c r="L21" s="13"/>
@@ -5462,26 +5463,26 @@
       <c r="C22" s="13">
         <v>14</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D22" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E22" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="13" t="s">
-        <v>23</v>
-      </c>
       <c r="F22" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H22" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K22" s="13"/>
       <c r="L22" s="13"/>
@@ -5510,26 +5511,26 @@
       <c r="C23" s="14">
         <v>16</v>
       </c>
-      <c r="D23" s="14" t="s">
+      <c r="D23" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E23" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="E23" s="14" t="s">
-        <v>23</v>
-      </c>
       <c r="F23" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G23" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H23" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J23" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K23" s="14"/>
       <c r="L23" s="14"/>
@@ -5614,22 +5615,22 @@
       <c r="AC25" s="42"/>
     </row>
     <row r="26" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B26" s="49" t="s">
-        <v>62</v>
-      </c>
-      <c r="C26" s="50"/>
-      <c r="D26" s="50"/>
-      <c r="E26" s="50"/>
-      <c r="F26" s="50"/>
+      <c r="B26" s="68" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="69"/>
+      <c r="D26" s="69"/>
+      <c r="E26" s="69"/>
+      <c r="F26" s="69"/>
       <c r="G26" s="18">
         <f>IF(SUM(K26:AA26)=0,"",SUM(K26:AA26))</f>
         <v>16.800000000000004</v>
       </c>
-      <c r="H26" s="50" t="s">
-        <v>49</v>
-      </c>
-      <c r="I26" s="50"/>
-      <c r="J26" s="50"/>
+      <c r="H26" s="69" t="s">
+        <v>48</v>
+      </c>
+      <c r="I26" s="69"/>
+      <c r="J26" s="69"/>
       <c r="K26" s="18" t="str">
         <f>IF(SUM(K5:K25)=0,"",SUM(K5:K25))</f>
         <v/>
@@ -5708,22 +5709,22 @@
       </c>
     </row>
     <row r="27" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B27" s="51" t="s">
-        <v>63</v>
-      </c>
-      <c r="C27" s="52"/>
-      <c r="D27" s="52"/>
-      <c r="E27" s="52"/>
-      <c r="F27" s="52"/>
+      <c r="B27" s="70" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" s="71"/>
+      <c r="D27" s="71"/>
+      <c r="E27" s="71"/>
+      <c r="F27" s="71"/>
       <c r="G27" s="19">
         <f>IF(SUM(K28:AA28)=0,"",SUM(K28:AA28))</f>
         <v>47.1</v>
       </c>
-      <c r="H27" s="55" t="s">
-        <v>61</v>
-      </c>
-      <c r="I27" s="55"/>
-      <c r="J27" s="55"/>
+      <c r="H27" s="74" t="s">
+        <v>60</v>
+      </c>
+      <c r="I27" s="74"/>
+      <c r="J27" s="74"/>
       <c r="K27" s="19" t="str">
         <f>'Page 02'!K28</f>
         <v/>
@@ -5802,22 +5803,22 @@
       </c>
     </row>
     <row r="28" spans="2:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="53" t="s">
-        <v>64</v>
-      </c>
-      <c r="C28" s="54"/>
-      <c r="D28" s="54"/>
-      <c r="E28" s="54"/>
-      <c r="F28" s="54"/>
+      <c r="B28" s="72" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="73"/>
+      <c r="D28" s="73"/>
+      <c r="E28" s="73"/>
+      <c r="F28" s="73"/>
       <c r="G28" s="45">
         <f>IF(SUM(G27,AC28)=0, "", SUM(G27,AC28))</f>
         <v>47.1</v>
       </c>
-      <c r="H28" s="54" t="s">
-        <v>50</v>
-      </c>
-      <c r="I28" s="54"/>
-      <c r="J28" s="54"/>
+      <c r="H28" s="73" t="s">
+        <v>49</v>
+      </c>
+      <c r="I28" s="73"/>
+      <c r="J28" s="73"/>
       <c r="K28" s="45" t="str">
         <f>IF(SUM(K26:K27)=0,"",SUM(K26:K27))</f>
         <v/>
@@ -5897,15 +5898,12 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="D2:E3"/>
-    <mergeCell ref="F2:F4"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="H2:J3"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="H26:J26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="H27:J27"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="H28:J28"/>
     <mergeCell ref="N3:O3"/>
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="AC3:AC4"/>
@@ -5919,12 +5917,15 @@
     <mergeCell ref="X3:Y3"/>
     <mergeCell ref="Z3:AA3"/>
     <mergeCell ref="AB3:AB4"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="H26:J26"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="H27:J27"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="H28:J28"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="D2:E3"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="H2:J3"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="M3:M4"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5939,9 +5940,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E13AED63-1410-A341-9CF8-EFDD2A09DD73}">
   <dimension ref="B1:AC28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5960,98 +5959,98 @@
   <sheetData>
     <row r="1" spans="2:29" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B2" s="83" t="s">
-        <v>81</v>
-      </c>
-      <c r="C2" s="84"/>
-      <c r="D2" s="87" t="s">
+      <c r="B2" s="75" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="76"/>
+      <c r="D2" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="84"/>
-      <c r="F2" s="89" t="s">
+      <c r="E2" s="76"/>
+      <c r="F2" s="81" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="89" t="s">
+      <c r="G2" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="87" t="s">
+      <c r="H2" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="92"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="64" t="s">
+      <c r="I2" s="84"/>
+      <c r="J2" s="76"/>
+      <c r="K2" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="65"/>
-      <c r="M2" s="66"/>
-      <c r="N2" s="60" t="s">
+      <c r="L2" s="50"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="79"/>
-      <c r="P2" s="79"/>
-      <c r="Q2" s="79"/>
-      <c r="R2" s="79"/>
-      <c r="S2" s="61"/>
-      <c r="T2" s="60" t="s">
+      <c r="O2" s="92"/>
+      <c r="P2" s="92"/>
+      <c r="Q2" s="92"/>
+      <c r="R2" s="92"/>
+      <c r="S2" s="65"/>
+      <c r="T2" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="U2" s="79"/>
-      <c r="V2" s="79"/>
-      <c r="W2" s="79"/>
-      <c r="X2" s="79"/>
-      <c r="Y2" s="61"/>
-      <c r="Z2" s="60"/>
-      <c r="AA2" s="61"/>
-      <c r="AB2" s="60" t="s">
+      <c r="U2" s="92"/>
+      <c r="V2" s="92"/>
+      <c r="W2" s="92"/>
+      <c r="X2" s="92"/>
+      <c r="Y2" s="65"/>
+      <c r="Z2" s="64"/>
+      <c r="AA2" s="65"/>
+      <c r="AB2" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="AC2" s="80"/>
+      <c r="AC2" s="93"/>
     </row>
     <row r="3" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B3" s="85"/>
-      <c r="C3" s="86"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="88"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="86"/>
-      <c r="K3" s="94"/>
-      <c r="L3" s="94"/>
-      <c r="M3" s="94"/>
-      <c r="N3" s="75" t="s">
+      <c r="B3" s="77"/>
+      <c r="C3" s="78"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="78"/>
+      <c r="K3" s="86"/>
+      <c r="L3" s="86"/>
+      <c r="M3" s="86"/>
+      <c r="N3" s="88" t="s">
         <v>9</v>
       </c>
-      <c r="O3" s="76"/>
-      <c r="P3" s="75" t="s">
+      <c r="O3" s="89"/>
+      <c r="P3" s="88" t="s">
         <v>12</v>
       </c>
-      <c r="Q3" s="76"/>
-      <c r="R3" s="75" t="s">
+      <c r="Q3" s="89"/>
+      <c r="R3" s="88" t="s">
         <v>13</v>
       </c>
-      <c r="S3" s="76"/>
-      <c r="T3" s="75" t="s">
+      <c r="S3" s="89"/>
+      <c r="T3" s="88" t="s">
         <v>9</v>
       </c>
-      <c r="U3" s="76"/>
-      <c r="V3" s="75" t="s">
+      <c r="U3" s="89"/>
+      <c r="V3" s="88" t="s">
         <v>12</v>
       </c>
-      <c r="W3" s="76"/>
-      <c r="X3" s="75" t="s">
+      <c r="W3" s="89"/>
+      <c r="X3" s="88" t="s">
         <v>13</v>
       </c>
-      <c r="Y3" s="76"/>
-      <c r="Z3" s="75" t="s">
+      <c r="Y3" s="89"/>
+      <c r="Z3" s="88" t="s">
         <v>16</v>
       </c>
-      <c r="AA3" s="76"/>
-      <c r="AB3" s="81" t="s">
+      <c r="AA3" s="89"/>
+      <c r="AB3" s="94" t="s">
         <v>18</v>
       </c>
-      <c r="AC3" s="77" t="s">
+      <c r="AC3" s="90" t="s">
         <v>19</v>
       </c>
     </row>
@@ -6068,20 +6067,20 @@
       <c r="E4" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="91"/>
-      <c r="G4" s="91"/>
+      <c r="F4" s="83"/>
+      <c r="G4" s="83"/>
       <c r="H4" s="21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I4" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="J4" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="K4" s="95"/>
-      <c r="L4" s="95"/>
-      <c r="M4" s="95"/>
+      <c r="K4" s="87"/>
+      <c r="L4" s="87"/>
+      <c r="M4" s="87"/>
       <c r="N4" s="20" t="s">
         <v>10</v>
       </c>
@@ -6124,36 +6123,36 @@
       <c r="AA4" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="AB4" s="82"/>
-      <c r="AC4" s="78"/>
+      <c r="AB4" s="95"/>
+      <c r="AC4" s="91"/>
     </row>
     <row r="5" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B5" s="37" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C5" s="1">
         <v>28</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -6179,31 +6178,31 @@
     </row>
     <row r="6" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B6" s="32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" s="13">
         <v>2</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E6" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="13" t="s">
-        <v>23</v>
-      </c>
       <c r="F6" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="G6" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="H6" s="13" t="s">
-        <v>91</v>
-      </c>
       <c r="I6" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K6" s="13"/>
       <c r="L6" s="13"/>
@@ -6232,26 +6231,26 @@
       <c r="C7" s="13">
         <v>8</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E7" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="13" t="s">
-        <v>23</v>
-      </c>
       <c r="F7" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K7" s="13"/>
       <c r="L7" s="13"/>
@@ -6280,26 +6279,26 @@
       <c r="C8" s="13">
         <v>9</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E8" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="13" t="s">
-        <v>23</v>
-      </c>
       <c r="F8" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K8" s="13"/>
       <c r="L8" s="13"/>
@@ -6328,26 +6327,26 @@
       <c r="C9" s="13">
         <v>11</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="13" t="s">
-        <v>23</v>
-      </c>
       <c r="F9" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K9" s="13"/>
       <c r="L9" s="13"/>
@@ -6373,31 +6372,31 @@
     </row>
     <row r="10" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B10" s="32" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C10" s="13">
         <v>18</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E10" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="13" t="s">
-        <v>23</v>
-      </c>
       <c r="F10" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K10" s="13"/>
       <c r="L10" s="13"/>
@@ -6426,26 +6425,26 @@
       <c r="C11" s="13">
         <v>28</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E11" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="13" t="s">
-        <v>23</v>
-      </c>
       <c r="F11" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K11" s="13"/>
       <c r="L11" s="13"/>
@@ -6471,31 +6470,31 @@
     </row>
     <row r="12" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B12" s="32" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C12" s="13">
         <v>2</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E12" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="13" t="s">
-        <v>23</v>
-      </c>
       <c r="F12" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="G12" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="H12" s="13" t="s">
-        <v>98</v>
-      </c>
       <c r="I12" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K12" s="13"/>
       <c r="L12" s="13"/>
@@ -6526,26 +6525,26 @@
       <c r="C13" s="13">
         <v>15</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E13" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="13" t="s">
-        <v>23</v>
-      </c>
       <c r="F13" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="G13" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="H13" s="13" t="s">
-        <v>100</v>
-      </c>
       <c r="I13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K13" s="13"/>
       <c r="L13" s="13"/>
@@ -6930,22 +6929,22 @@
       <c r="AC25" s="42"/>
     </row>
     <row r="26" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B26" s="49" t="s">
-        <v>62</v>
-      </c>
-      <c r="C26" s="50"/>
-      <c r="D26" s="50"/>
-      <c r="E26" s="50"/>
-      <c r="F26" s="50"/>
+      <c r="B26" s="68" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="69"/>
+      <c r="D26" s="69"/>
+      <c r="E26" s="69"/>
+      <c r="F26" s="69"/>
       <c r="G26" s="18">
         <f>IF(SUM(K26:AA26)=0,"",SUM(K26:AA26))</f>
         <v>9.7999999999999989</v>
       </c>
-      <c r="H26" s="50" t="s">
-        <v>49</v>
-      </c>
-      <c r="I26" s="50"/>
-      <c r="J26" s="50"/>
+      <c r="H26" s="69" t="s">
+        <v>48</v>
+      </c>
+      <c r="I26" s="69"/>
+      <c r="J26" s="69"/>
       <c r="K26" s="18" t="str">
         <f>IF(SUM(K5:K25)=0,"",SUM(K5:K25))</f>
         <v/>
@@ -7024,22 +7023,22 @@
       </c>
     </row>
     <row r="27" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B27" s="51" t="s">
-        <v>63</v>
-      </c>
-      <c r="C27" s="52"/>
-      <c r="D27" s="52"/>
-      <c r="E27" s="52"/>
-      <c r="F27" s="52"/>
+      <c r="B27" s="70" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" s="71"/>
+      <c r="D27" s="71"/>
+      <c r="E27" s="71"/>
+      <c r="F27" s="71"/>
       <c r="G27" s="19">
         <f>IF(SUM(K28:AA28)=0,"",SUM(K28:AA28))</f>
         <v>56.9</v>
       </c>
-      <c r="H27" s="55" t="s">
-        <v>61</v>
-      </c>
-      <c r="I27" s="55"/>
-      <c r="J27" s="55"/>
+      <c r="H27" s="74" t="s">
+        <v>60</v>
+      </c>
+      <c r="I27" s="74"/>
+      <c r="J27" s="74"/>
       <c r="K27" s="19" t="str">
         <f>'Page 03'!K28</f>
         <v/>
@@ -7118,22 +7117,22 @@
       </c>
     </row>
     <row r="28" spans="2:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="53" t="s">
-        <v>64</v>
-      </c>
-      <c r="C28" s="54"/>
-      <c r="D28" s="54"/>
-      <c r="E28" s="54"/>
-      <c r="F28" s="54"/>
+      <c r="B28" s="72" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="73"/>
+      <c r="D28" s="73"/>
+      <c r="E28" s="73"/>
+      <c r="F28" s="73"/>
       <c r="G28" s="45">
         <f>IF(SUM(G27,AC28)=0, "", SUM(G27,AC28))</f>
         <v>56.9</v>
       </c>
-      <c r="H28" s="54" t="s">
-        <v>50</v>
-      </c>
-      <c r="I28" s="54"/>
-      <c r="J28" s="54"/>
+      <c r="H28" s="73" t="s">
+        <v>49</v>
+      </c>
+      <c r="I28" s="73"/>
+      <c r="J28" s="73"/>
       <c r="K28" s="45" t="str">
         <f>IF(SUM(K26:K27)=0,"",SUM(K26:K27))</f>
         <v/>
@@ -7213,15 +7212,12 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="D2:E3"/>
-    <mergeCell ref="F2:F4"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="H2:J3"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="H26:J26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="H27:J27"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="H28:J28"/>
     <mergeCell ref="N3:O3"/>
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="AC3:AC4"/>
@@ -7235,12 +7231,15 @@
     <mergeCell ref="X3:Y3"/>
     <mergeCell ref="Z3:AA3"/>
     <mergeCell ref="AB3:AB4"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="H26:J26"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="H27:J27"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="H28:J28"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="D2:E3"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="H2:J3"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="M3:M4"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7273,98 +7272,98 @@
   <sheetData>
     <row r="1" spans="2:29" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B2" s="83" t="s">
-        <v>60</v>
-      </c>
-      <c r="C2" s="84"/>
-      <c r="D2" s="87" t="s">
+      <c r="B2" s="75" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="76"/>
+      <c r="D2" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="84"/>
-      <c r="F2" s="89" t="s">
+      <c r="E2" s="76"/>
+      <c r="F2" s="81" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="89" t="s">
+      <c r="G2" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="87" t="s">
+      <c r="H2" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="92"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="64" t="s">
+      <c r="I2" s="84"/>
+      <c r="J2" s="76"/>
+      <c r="K2" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="65"/>
-      <c r="M2" s="66"/>
-      <c r="N2" s="60" t="s">
+      <c r="L2" s="50"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="79"/>
-      <c r="P2" s="79"/>
-      <c r="Q2" s="79"/>
-      <c r="R2" s="79"/>
-      <c r="S2" s="61"/>
-      <c r="T2" s="60" t="s">
+      <c r="O2" s="92"/>
+      <c r="P2" s="92"/>
+      <c r="Q2" s="92"/>
+      <c r="R2" s="92"/>
+      <c r="S2" s="65"/>
+      <c r="T2" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="U2" s="79"/>
-      <c r="V2" s="79"/>
-      <c r="W2" s="79"/>
-      <c r="X2" s="79"/>
-      <c r="Y2" s="61"/>
-      <c r="Z2" s="60"/>
-      <c r="AA2" s="61"/>
-      <c r="AB2" s="60" t="s">
+      <c r="U2" s="92"/>
+      <c r="V2" s="92"/>
+      <c r="W2" s="92"/>
+      <c r="X2" s="92"/>
+      <c r="Y2" s="65"/>
+      <c r="Z2" s="64"/>
+      <c r="AA2" s="65"/>
+      <c r="AB2" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="AC2" s="80"/>
+      <c r="AC2" s="93"/>
     </row>
     <row r="3" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B3" s="85"/>
-      <c r="C3" s="86"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="88"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="86"/>
-      <c r="K3" s="94"/>
-      <c r="L3" s="94"/>
-      <c r="M3" s="94"/>
-      <c r="N3" s="75" t="s">
+      <c r="B3" s="77"/>
+      <c r="C3" s="78"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="78"/>
+      <c r="K3" s="86"/>
+      <c r="L3" s="86"/>
+      <c r="M3" s="86"/>
+      <c r="N3" s="88" t="s">
         <v>9</v>
       </c>
-      <c r="O3" s="76"/>
-      <c r="P3" s="75" t="s">
+      <c r="O3" s="89"/>
+      <c r="P3" s="88" t="s">
         <v>12</v>
       </c>
-      <c r="Q3" s="76"/>
-      <c r="R3" s="75" t="s">
+      <c r="Q3" s="89"/>
+      <c r="R3" s="88" t="s">
         <v>13</v>
       </c>
-      <c r="S3" s="76"/>
-      <c r="T3" s="75" t="s">
+      <c r="S3" s="89"/>
+      <c r="T3" s="88" t="s">
         <v>9</v>
       </c>
-      <c r="U3" s="76"/>
-      <c r="V3" s="75" t="s">
+      <c r="U3" s="89"/>
+      <c r="V3" s="88" t="s">
         <v>12</v>
       </c>
-      <c r="W3" s="76"/>
-      <c r="X3" s="75" t="s">
+      <c r="W3" s="89"/>
+      <c r="X3" s="88" t="s">
         <v>13</v>
       </c>
-      <c r="Y3" s="76"/>
-      <c r="Z3" s="75" t="s">
+      <c r="Y3" s="89"/>
+      <c r="Z3" s="88" t="s">
         <v>16</v>
       </c>
-      <c r="AA3" s="76"/>
-      <c r="AB3" s="81" t="s">
+      <c r="AA3" s="89"/>
+      <c r="AB3" s="94" t="s">
         <v>18</v>
       </c>
-      <c r="AC3" s="77" t="s">
+      <c r="AC3" s="90" t="s">
         <v>19</v>
       </c>
     </row>
@@ -7381,20 +7380,20 @@
       <c r="E4" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="91"/>
-      <c r="G4" s="91"/>
+      <c r="F4" s="83"/>
+      <c r="G4" s="83"/>
       <c r="H4" s="21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I4" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="J4" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="K4" s="95"/>
-      <c r="L4" s="95"/>
-      <c r="M4" s="95"/>
+      <c r="K4" s="87"/>
+      <c r="L4" s="87"/>
+      <c r="M4" s="87"/>
       <c r="N4" s="20" t="s">
         <v>10</v>
       </c>
@@ -7437,8 +7436,8 @@
       <c r="AA4" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="AB4" s="82"/>
-      <c r="AC4" s="78"/>
+      <c r="AB4" s="95"/>
+      <c r="AC4" s="91"/>
     </row>
     <row r="5" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B5" s="37"/>
@@ -8071,22 +8070,22 @@
       <c r="AC25" s="42"/>
     </row>
     <row r="26" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B26" s="49" t="s">
-        <v>62</v>
-      </c>
-      <c r="C26" s="50"/>
-      <c r="D26" s="50"/>
-      <c r="E26" s="50"/>
-      <c r="F26" s="50"/>
+      <c r="B26" s="68" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="69"/>
+      <c r="D26" s="69"/>
+      <c r="E26" s="69"/>
+      <c r="F26" s="69"/>
       <c r="G26" s="18" t="str">
         <f>IF(SUM(K26:AA26)=0,"",SUM(K26:AA26))</f>
         <v/>
       </c>
-      <c r="H26" s="50" t="s">
-        <v>49</v>
-      </c>
-      <c r="I26" s="50"/>
-      <c r="J26" s="50"/>
+      <c r="H26" s="69" t="s">
+        <v>48</v>
+      </c>
+      <c r="I26" s="69"/>
+      <c r="J26" s="69"/>
       <c r="K26" s="18" t="str">
         <f>IF(SUM(K5:K25)=0,"",SUM(K5:K25))</f>
         <v/>
@@ -8165,22 +8164,22 @@
       </c>
     </row>
     <row r="27" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B27" s="51" t="s">
-        <v>63</v>
-      </c>
-      <c r="C27" s="52"/>
-      <c r="D27" s="52"/>
-      <c r="E27" s="52"/>
-      <c r="F27" s="52"/>
+      <c r="B27" s="70" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" s="71"/>
+      <c r="D27" s="71"/>
+      <c r="E27" s="71"/>
+      <c r="F27" s="71"/>
       <c r="G27" s="19">
         <f>IF(SUM(K28:AA28)=0,"",SUM(K28:AA28))</f>
         <v>56.9</v>
       </c>
-      <c r="H27" s="55" t="s">
-        <v>61</v>
-      </c>
-      <c r="I27" s="55"/>
-      <c r="J27" s="55"/>
+      <c r="H27" s="74" t="s">
+        <v>60</v>
+      </c>
+      <c r="I27" s="74"/>
+      <c r="J27" s="74"/>
       <c r="K27" s="19" t="str">
         <f>'Page 04'!K28</f>
         <v/>
@@ -8259,22 +8258,22 @@
       </c>
     </row>
     <row r="28" spans="2:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="53" t="s">
-        <v>64</v>
-      </c>
-      <c r="C28" s="54"/>
-      <c r="D28" s="54"/>
-      <c r="E28" s="54"/>
-      <c r="F28" s="54"/>
+      <c r="B28" s="72" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="73"/>
+      <c r="D28" s="73"/>
+      <c r="E28" s="73"/>
+      <c r="F28" s="73"/>
       <c r="G28" s="45">
         <f>IF(SUM(G27,AC28)=0, "", SUM(G27,AC28))</f>
         <v>56.9</v>
       </c>
-      <c r="H28" s="54" t="s">
-        <v>50</v>
-      </c>
-      <c r="I28" s="54"/>
-      <c r="J28" s="54"/>
+      <c r="H28" s="73" t="s">
+        <v>49</v>
+      </c>
+      <c r="I28" s="73"/>
+      <c r="J28" s="73"/>
       <c r="K28" s="45" t="str">
         <f>IF(SUM(K26:K27)=0,"",SUM(K26:K27))</f>
         <v/>
@@ -8354,15 +8353,12 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="D2:E3"/>
-    <mergeCell ref="F2:F4"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="H2:J3"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="H26:J26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="H27:J27"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="H28:J28"/>
     <mergeCell ref="N3:O3"/>
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="AC3:AC4"/>
@@ -8376,12 +8372,15 @@
     <mergeCell ref="X3:Y3"/>
     <mergeCell ref="Z3:AA3"/>
     <mergeCell ref="AB3:AB4"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="H26:J26"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="H27:J27"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="H28:J28"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="D2:E3"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="H2:J3"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="M3:M4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="86" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>